<commit_message>
added default routes to switch
</commit_message>
<xml_diff>
--- a/CLI.xlsx
+++ b/CLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxim\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EEE52B-0A18-446A-9034-FDF307CEC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A6B675-D167-47EA-988B-639B156CE125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{34B683BC-2245-4D05-9364-220B19A460DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{34B683BC-2245-4D05-9364-220B19A460DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Router" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="142">
   <si>
     <t>RT-HH-01</t>
   </si>
@@ -451,6 +451,18 @@
   </si>
   <si>
     <t>ipv6 route 2001:db8:C50::/64 fd00:CAFE:CD::1</t>
+  </si>
+  <si>
+    <t>ipv6 route ::/0 fd00:CAFE:AA::1</t>
+  </si>
+  <si>
+    <t>ipv6 route ::/0 fd00:CAFE:BB::1</t>
+  </si>
+  <si>
+    <t>ipv6 route ::/0 fd00:CAFE:CC::1</t>
+  </si>
+  <si>
+    <t>ipv6 route ::/0 fd00:CAFE:DD::1</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -630,6 +642,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -638,9 +656,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF001F32"/>
       <color rgb="FF00273E"/>
       <color rgb="FFF5F5F5"/>
+      <color rgb="FF001F32"/>
       <color rgb="FF1C50A6"/>
     </mruColors>
   </colors>
@@ -974,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E81B47-BD4C-4A16-B0C6-3253E569DD17}">
   <dimension ref="A1:AJ44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:D43"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2605,11 +2623,11 @@
       <c r="AB34" s="16"/>
       <c r="AC34" s="16"/>
       <c r="AD34" s="16"/>
-      <c r="AE34" s="16"/>
+      <c r="AE34" s="24"/>
       <c r="AF34" s="19"/>
-      <c r="AG34" s="16"/>
-      <c r="AH34" s="16"/>
-      <c r="AI34" s="16"/>
+      <c r="AG34" s="25"/>
+      <c r="AH34" s="25"/>
+      <c r="AI34" s="25"/>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
@@ -3197,10 +3215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC194F1D-C6D7-4472-AAD1-B0F01E2CC6D9}">
-  <dimension ref="A1:AI45"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView topLeftCell="L9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AE30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37:M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4304,14 +4322,22 @@
       <c r="O26" s="16"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="15"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AD26" s="14"/>
-      <c r="AE26" s="15"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="16"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -4338,15 +4364,15 @@
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
+      <c r="S27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V27" s="26"/>
       <c r="W27" s="11"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="14"/>
+      <c r="AB27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="26"/>
       <c r="AF27" s="11"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
@@ -4374,20 +4400,22 @@
       <c r="O28" s="14"/>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
-      <c r="S28" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="11"/>
-      <c r="AB28" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC28" s="14"/>
-      <c r="AD28" s="14"/>
-      <c r="AE28" s="14"/>
-      <c r="AF28" s="11"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AB28" s="16"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="12"/>
+      <c r="AI28" s="12"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
@@ -4414,15 +4442,19 @@
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
-      <c r="S29" s="14"/>
+      <c r="S29" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="T29" s="14"/>
       <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
+      <c r="V29" s="15"/>
       <c r="W29" s="11"/>
-      <c r="AB29" s="14"/>
+      <c r="AB29" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="AC29" s="14"/>
       <c r="AD29" s="14"/>
-      <c r="AE29" s="14"/>
+      <c r="AE29" s="15"/>
       <c r="AF29" s="11"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
@@ -4442,22 +4474,22 @@
       <c r="O30" s="16"/>
       <c r="P30" s="16"/>
       <c r="Q30" s="16"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="14"/>
-      <c r="Z30" s="14"/>
-      <c r="AB30" s="14"/>
-      <c r="AC30" s="14"/>
-      <c r="AD30" s="14"/>
-      <c r="AE30" s="14"/>
-      <c r="AF30" s="14"/>
-      <c r="AG30" s="14"/>
-      <c r="AH30" s="14"/>
-      <c r="AI30" s="14"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
@@ -4484,22 +4516,20 @@
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="S31" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
-      <c r="Z31" s="14"/>
-      <c r="AB31" s="14"/>
+      <c r="W31" s="11"/>
+      <c r="AB31" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="AC31" s="14"/>
       <c r="AD31" s="14"/>
       <c r="AE31" s="14"/>
-      <c r="AF31" s="14"/>
-      <c r="AG31" s="14"/>
-      <c r="AH31" s="14"/>
-      <c r="AI31" s="14"/>
+      <c r="AF31" s="11"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
@@ -4530,18 +4560,12 @@
       <c r="T32" s="14"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="14"/>
-      <c r="Z32" s="14"/>
+      <c r="W32" s="11"/>
       <c r="AB32" s="14"/>
       <c r="AC32" s="14"/>
       <c r="AD32" s="14"/>
       <c r="AE32" s="14"/>
-      <c r="AF32" s="14"/>
-      <c r="AG32" s="14"/>
-      <c r="AH32" s="14"/>
-      <c r="AI32" s="14"/>
+      <c r="AF32" s="11"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
@@ -4586,14 +4610,22 @@
       <c r="AI33" s="14"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="15"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
       <c r="U34" s="14"/>
@@ -4604,62 +4636,96 @@
       <c r="AE34" s="14"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="26"/>
       <c r="E35" s="11"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
+      <c r="J35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="26"/>
       <c r="N35" s="11"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="11"/>
-      <c r="J36" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="11"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="11"/>
-      <c r="J37" s="14"/>
+      <c r="J37" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
+      <c r="M37" s="15"/>
       <c r="N37" s="11"/>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
+      <c r="E39" s="11"/>
+      <c r="J39" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="11"/>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
+      <c r="E40" s="11"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="11"/>
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
@@ -4691,11 +4757,31 @@
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="264">
-    <mergeCell ref="J35:M35"/>
+  <mergeCells count="256">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="J37:M37"/>
     <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
     <mergeCell ref="AB1:AI1"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="AF2:AI2"/>
@@ -4720,13 +4806,8 @@
     <mergeCell ref="AF17:AI17"/>
     <mergeCell ref="AF18:AI18"/>
     <mergeCell ref="AB34:AE34"/>
-    <mergeCell ref="AB30:AE30"/>
-    <mergeCell ref="AF30:AI30"/>
     <mergeCell ref="AB31:AE31"/>
-    <mergeCell ref="AF31:AI31"/>
     <mergeCell ref="AB32:AE32"/>
-    <mergeCell ref="AF32:AI32"/>
-    <mergeCell ref="AB27:AE27"/>
     <mergeCell ref="AB28:AE28"/>
     <mergeCell ref="AB29:AE29"/>
     <mergeCell ref="AF19:AI19"/>
@@ -4754,7 +4835,6 @@
     <mergeCell ref="W33:Z33"/>
     <mergeCell ref="S34:V34"/>
     <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:Z32"/>
     <mergeCell ref="S18:V18"/>
     <mergeCell ref="W18:Z18"/>
     <mergeCell ref="S19:V19"/>
@@ -4774,11 +4854,7 @@
     <mergeCell ref="AF6:AI6"/>
     <mergeCell ref="AB7:AE7"/>
     <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="S30:V30"/>
-    <mergeCell ref="W30:Z30"/>
     <mergeCell ref="S31:V31"/>
-    <mergeCell ref="W31:Z31"/>
-    <mergeCell ref="S27:V27"/>
     <mergeCell ref="S28:V28"/>
     <mergeCell ref="S29:V29"/>
     <mergeCell ref="S24:V24"/>
@@ -4900,7 +4976,7 @@
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="E5:H5"/>
@@ -4909,18 +4985,18 @@
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="E11:H11"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:D38"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A28:D28"/>
@@ -4959,5 +5035,6 @@
     <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added OSPFv3 to Switches
</commit_message>
<xml_diff>
--- a/CLI.xlsx
+++ b/CLI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxim\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289DE64C-25F5-40FA-AD5F-6449F1E48DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E69848-E000-4908-87E0-79462E344C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{34B683BC-2245-4D05-9364-220B19A460DB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="177">
   <si>
     <t>RT-HH-01</t>
   </si>
@@ -558,6 +558,18 @@
   </si>
   <si>
     <t>ipv6 ospf 1 area 4</t>
+  </si>
+  <si>
+    <t>router-id 1.1.2.1</t>
+  </si>
+  <si>
+    <t>router-id 1.1.2.2</t>
+  </si>
+  <si>
+    <t>router-id 1.1.2.3</t>
+  </si>
+  <si>
+    <t>router-id 1.1.2.4</t>
   </si>
 </sst>
 </file>
@@ -5963,8 +5975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF66C8F-F7E7-4E47-AB56-867EE702083D}">
   <dimension ref="A1:AJ54"/>
   <sheetViews>
-    <sheetView topLeftCell="M30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB45" sqref="AB45:AE45"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -8570,10 +8582,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D58D888-97B0-4BB4-B0DF-40F9EA743ADA}">
-  <dimension ref="A1:AI52"/>
+  <dimension ref="A1:AI59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z41" sqref="Z41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB31" sqref="AB31:AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -9135,316 +9147,278 @@
       <c r="AI13" s="15"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="J14" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="S14" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AB14" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="16"/>
-      <c r="AF14" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG14" s="15"/>
-      <c r="AH14" s="15"/>
-      <c r="AI14" s="15"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="12"/>
+      <c r="AI14" s="12"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="E15" s="11"/>
       <c r="J15" s="15" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
+      <c r="N15" s="11"/>
       <c r="S15" s="15" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
       <c r="V15" s="16"/>
-      <c r="W15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
+      <c r="W15" s="11"/>
       <c r="AB15" s="15" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
       <c r="AE15" s="16"/>
-      <c r="AF15" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
+      <c r="AF15" s="11"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="E16" s="11"/>
       <c r="J16" s="15" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
+      <c r="N16" s="11"/>
       <c r="S16" s="15" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
       <c r="V16" s="16"/>
-      <c r="W16" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
+      <c r="W16" s="11"/>
       <c r="AB16" s="15" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="AC16" s="15"/>
       <c r="AD16" s="15"/>
       <c r="AE16" s="16"/>
-      <c r="AF16" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="AG16" s="15"/>
-      <c r="AH16" s="15"/>
-      <c r="AI16" s="15"/>
+      <c r="AF16" s="11"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="J17" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="S17" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AB17" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="16"/>
-      <c r="AF17" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="AG17" s="15"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="12"/>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="12"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="20"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="20"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
+      <c r="A18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="J18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="S18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AB18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="16"/>
+      <c r="AF18" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="A19" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="17" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="J19" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="J19" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="16"/>
       <c r="N19" s="17" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
       <c r="S19" s="15" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
       <c r="V19" s="16"/>
       <c r="W19" s="17" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
-      <c r="AB19" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="AB19" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="16"/>
       <c r="AF19" s="17" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="AG19" s="15"/>
       <c r="AH19" s="15"/>
       <c r="AI19" s="15"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A20" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="17" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="J20" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="J20" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="16"/>
       <c r="N20" s="17" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="S20" s="15" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
       <c r="V20" s="16"/>
       <c r="W20" s="17" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="X20" s="15"/>
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
-      <c r="AB20" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="AB20" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="16"/>
       <c r="AF20" s="17" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AG20" s="15"/>
       <c r="AH20" s="15"/>
@@ -9452,49 +9426,49 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="17" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="J21" s="15" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="M21" s="16"/>
       <c r="N21" s="17" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="S21" s="15" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="T21" s="15"/>
       <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
+      <c r="V21" s="16"/>
       <c r="W21" s="17" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
       <c r="AB21" s="15" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
+      <c r="AE21" s="16"/>
       <c r="AF21" s="17" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="AG21" s="15"/>
       <c r="AH21" s="15"/>
@@ -9504,7 +9478,7 @@
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
-      <c r="D22" s="21"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="20"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
@@ -9512,7 +9486,7 @@
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="18"/>
       <c r="N22" s="20"/>
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
@@ -9520,7 +9494,7 @@
       <c r="S22" s="18"/>
       <c r="T22" s="18"/>
       <c r="U22" s="18"/>
-      <c r="V22" s="21"/>
+      <c r="V22" s="18"/>
       <c r="W22" s="20"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="18"/>
@@ -9528,107 +9502,89 @@
       <c r="AB22" s="18"/>
       <c r="AC22" s="18"/>
       <c r="AD22" s="18"/>
-      <c r="AE22" s="21"/>
+      <c r="AE22" s="18"/>
       <c r="AF22" s="20"/>
       <c r="AG22" s="18"/>
       <c r="AH22" s="18"/>
       <c r="AI22" s="18"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="E23" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="J23" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16"/>
+      <c r="J23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="N23" s="17" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
       <c r="S23" s="15" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
       <c r="V23" s="16"/>
       <c r="W23" s="17" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
-      <c r="AB23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="15"/>
-      <c r="AE23" s="16"/>
+      <c r="AB23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AF23" s="17" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="AG23" s="15"/>
       <c r="AH23" s="15"/>
       <c r="AI23" s="15"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
-      <c r="J24" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="J24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="N24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="S24" s="15" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
+      <c r="V24" s="16"/>
       <c r="W24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X24" s="15"/>
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
-      <c r="AB24" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
+      <c r="AB24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="AF24" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG24" s="15"/>
       <c r="AH24" s="15"/>
@@ -9636,183 +9592,166 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="J25" s="15" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="16"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="S25" s="15" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
-      <c r="V25" s="16"/>
+      <c r="V25" s="15"/>
       <c r="W25" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X25" s="15"/>
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
       <c r="AB25" s="15" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="AC25" s="15"/>
       <c r="AD25" s="15"/>
-      <c r="AE25" s="16"/>
+      <c r="AE25" s="15"/>
       <c r="AF25" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="18"/>
-      <c r="Z26" s="18"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
-      <c r="AD26" s="18"/>
-      <c r="AE26" s="21"/>
-      <c r="AF26" s="20"/>
-      <c r="AG26" s="18"/>
-      <c r="AH26" s="18"/>
-      <c r="AI26" s="18"/>
+      <c r="A26" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="J26" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="11"/>
+      <c r="S26" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="11"/>
+      <c r="AB26" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="11"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="J27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="S27" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-      <c r="AB27" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="15"/>
-      <c r="AE27" s="16"/>
-      <c r="AF27" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG27" s="15"/>
-      <c r="AH27" s="15"/>
-      <c r="AI27" s="15"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+      <c r="AB27" s="18"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="18"/>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="20"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="18"/>
+      <c r="AI27" s="18"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="J28" s="15" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="17" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
       <c r="S28" s="15" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
       <c r="V28" s="16"/>
       <c r="W28" s="17" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
       <c r="AB28" s="15" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="AC28" s="15"/>
       <c r="AD28" s="15"/>
       <c r="AE28" s="16"/>
       <c r="AF28" s="17" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="AG28" s="15"/>
       <c r="AH28" s="15"/>
@@ -9820,755 +9759,1132 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="J29" s="15" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
+      <c r="M29" s="15"/>
       <c r="N29" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
       <c r="S29" s="15" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="T29" s="15"/>
       <c r="U29" s="15"/>
-      <c r="V29" s="16"/>
+      <c r="V29" s="15"/>
       <c r="W29" s="17" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
       <c r="AB29" s="15" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="AC29" s="15"/>
       <c r="AD29" s="15"/>
-      <c r="AE29" s="16"/>
+      <c r="AE29" s="15"/>
       <c r="AF29" s="17" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="AG29" s="15"/>
       <c r="AH29" s="15"/>
       <c r="AI29" s="15"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="21"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="12"/>
-      <c r="Y30" s="12"/>
-      <c r="Z30" s="12"/>
-      <c r="AB30" s="18"/>
-      <c r="AC30" s="18"/>
-      <c r="AD30" s="18"/>
-      <c r="AE30" s="21"/>
-      <c r="AF30" s="12"/>
-      <c r="AG30" s="12"/>
-      <c r="AH30" s="12"/>
-      <c r="AI30" s="12"/>
+      <c r="A30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="J30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="S30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AB30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="16"/>
+      <c r="AF30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="J31" s="15" t="s">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="16"/>
-      <c r="N31" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="S31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W31" s="11"/>
-      <c r="AB31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF31" s="11"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="S31" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AB31" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC31" s="15"/>
+      <c r="AD31" s="15"/>
+      <c r="AE31" s="16"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="J32" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
       <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="12"/>
-      <c r="Y32" s="12"/>
-      <c r="Z32" s="12"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
       <c r="AB32" s="18"/>
       <c r="AC32" s="18"/>
       <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="12"/>
-      <c r="AH32" s="12"/>
-      <c r="AI32" s="12"/>
+      <c r="AE32" s="21"/>
+      <c r="AF32" s="20"/>
+      <c r="AG32" s="18"/>
+      <c r="AH32" s="18"/>
+      <c r="AI32" s="18"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
       <c r="E33" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="J33" s="15" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="16"/>
       <c r="N33" s="17" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="S33" s="15" t="s">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="T33" s="15"/>
       <c r="U33" s="15"/>
       <c r="V33" s="16"/>
-      <c r="W33" s="11"/>
+      <c r="W33" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
       <c r="AB33" s="15" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="AC33" s="15"/>
       <c r="AD33" s="15"/>
       <c r="AE33" s="16"/>
-      <c r="AF33" s="11"/>
+      <c r="AF33" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="15"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
-      <c r="U34" s="12"/>
-      <c r="V34" s="12"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="12"/>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-      <c r="AE34" s="12"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="12"/>
-      <c r="AH34" s="12"/>
-      <c r="AI34" s="12"/>
+      <c r="A34" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="J34" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="S34" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AB34" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="16"/>
+      <c r="AF34" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG34" s="15"/>
+      <c r="AH34" s="15"/>
+      <c r="AI34" s="15"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
       <c r="E35" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="16"/>
       <c r="N35" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
-      <c r="S35" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="5"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-      <c r="AB35" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="5"/>
-      <c r="AG35" s="2"/>
-      <c r="AH35" s="2"/>
-      <c r="AI35" s="2"/>
+      <c r="S35" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+      <c r="AB35" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC35" s="15"/>
+      <c r="AD35" s="15"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG35" s="15"/>
+      <c r="AH35" s="15"/>
+      <c r="AI35" s="15"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
-      <c r="E36" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
       <c r="J36" s="15" t="s">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="16"/>
-      <c r="N36" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="S36" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="N36" s="11"/>
+      <c r="S36" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="16"/>
       <c r="W36" s="5"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
-      <c r="AB36" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="AB36" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="16"/>
       <c r="AF36" s="5"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
+      <c r="AB37" s="18"/>
+      <c r="AC37" s="18"/>
+      <c r="AD37" s="18"/>
+      <c r="AE37" s="21"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="12"/>
+      <c r="AH37" s="12"/>
+      <c r="AI37" s="12"/>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="J38" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="S38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W38" s="11"/>
+      <c r="AB38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="11"/>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="J39" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+      <c r="V39" s="18"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="12"/>
+      <c r="Z39" s="12"/>
+      <c r="AB39" s="18"/>
+      <c r="AC39" s="18"/>
+      <c r="AD39" s="18"/>
+      <c r="AE39" s="18"/>
+      <c r="AF39" s="13"/>
+      <c r="AG39" s="12"/>
+      <c r="AH39" s="12"/>
+      <c r="AI39" s="12"/>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="J40" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="S40" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="11"/>
+      <c r="AB40" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="16"/>
+      <c r="AF40" s="11"/>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="12"/>
+      <c r="Z41" s="12"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="12"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="12"/>
+      <c r="AH41" s="12"/>
+      <c r="AI41" s="12"/>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="J42" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="S42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AB42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="5"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="J43" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="S43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="W43" s="5"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AB43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AI43" s="2"/>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="17" t="s">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="J37" s="15" t="s">
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="J44" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="17" t="s">
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="S37" s="15" t="s">
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="S44" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="5"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AB37" s="15" t="s">
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AB44" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="15"/>
-      <c r="AF37" s="5"/>
-      <c r="AG37" s="2"/>
-      <c r="AH37" s="2"/>
-      <c r="AI37" s="2"/>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
-      <c r="S38" s="1" t="s">
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="15"/>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
+      <c r="AI44" s="2"/>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="S45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="W38" s="5"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AB38" s="1" t="s">
+      <c r="W45" s="5"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AB45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AF38" s="5"/>
-      <c r="AG38" s="2"/>
-      <c r="AH38" s="2"/>
-      <c r="AI38" s="2"/>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="J39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N39" s="11"/>
-      <c r="S39" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="5"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AB39" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="AC39" s="15"/>
-      <c r="AD39" s="15"/>
-      <c r="AE39" s="15"/>
-      <c r="AF39" s="5"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="2"/>
-    </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="12"/>
-      <c r="S40" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="W40" s="5"/>
-      <c r="X40" s="2"/>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AB40" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AF40" s="5"/>
-      <c r="AG40" s="2"/>
-      <c r="AH40" s="2"/>
-      <c r="AI40" s="2"/>
-    </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="11"/>
-      <c r="J41" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="11"/>
-      <c r="S41" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="2"/>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AB41" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="5"/>
-      <c r="AG41" s="2"/>
-      <c r="AH41" s="2"/>
-      <c r="AI41" s="2"/>
-    </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="W42" s="11"/>
-      <c r="AF42" s="11"/>
-    </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="J43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-    </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="J44" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="N44" s="5"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-    </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="J45" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="2"/>
+      <c r="AH45" s="2"/>
+      <c r="AI45" s="2"/>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="11"/>
       <c r="J46" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="N46" s="5"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="N46" s="11"/>
+      <c r="S46" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AB46" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC46" s="15"/>
+      <c r="AD46" s="15"/>
+      <c r="AE46" s="15"/>
+      <c r="AF46" s="5"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="2"/>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="J47" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="S47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="W47" s="5"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AB47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2"/>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="J48" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N48" s="5"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A48" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="11"/>
+      <c r="J48" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="11"/>
+      <c r="S48" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="J49" s="15" t="s">
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+      <c r="AB48" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="11"/>
-      <c r="N50" s="11"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="AC48" s="15"/>
+      <c r="AD48" s="15"/>
+      <c r="AE48" s="15"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="2"/>
+      <c r="AH48" s="2"/>
+      <c r="AI48" s="2"/>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="W49" s="11"/>
+      <c r="AF49" s="11"/>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="J50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="J51" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N51" s="5"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>159</v>
+      </c>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="J52" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="J53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N53" s="5"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="J54" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="J55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="N55" s="5"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="J56" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="11"/>
+      <c r="N57" s="11"/>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="281">
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
+  <mergeCells count="301">
+    <mergeCell ref="AB31:AE31"/>
+    <mergeCell ref="AB36:AE36"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="AB26:AE26"/>
+    <mergeCell ref="S15:V15"/>
+    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="AB15:AE15"/>
+    <mergeCell ref="AB16:AE16"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="S31:V31"/>
+    <mergeCell ref="S36:V36"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
     <mergeCell ref="A52:D52"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="S48:V48"/>
+    <mergeCell ref="AB48:AE48"/>
+    <mergeCell ref="S44:V44"/>
+    <mergeCell ref="AB44:AE44"/>
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="J45:M45"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="S46:V46"/>
+    <mergeCell ref="AB46:AE46"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="A41:D41"/>
+    <mergeCell ref="E41:H41"/>
     <mergeCell ref="J41:M41"/>
-    <mergeCell ref="S41:V41"/>
-    <mergeCell ref="AB41:AE41"/>
-    <mergeCell ref="S37:V37"/>
-    <mergeCell ref="AB37:AE37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N41:Q41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="S39:V39"/>
     <mergeCell ref="AB39:AE39"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="S40:V40"/>
+    <mergeCell ref="AB40:AE40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N39:Q39"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="E37:H37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="S37:V37"/>
+    <mergeCell ref="AB37:AE37"/>
+    <mergeCell ref="AB34:AE34"/>
+    <mergeCell ref="AF34:AI34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="S35:V35"/>
+    <mergeCell ref="W35:Z35"/>
+    <mergeCell ref="AB35:AE35"/>
+    <mergeCell ref="AF35:AI35"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="E34:H34"/>
     <mergeCell ref="J34:M34"/>
     <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="S34:V34"/>
+    <mergeCell ref="W34:Z34"/>
     <mergeCell ref="AB32:AE32"/>
+    <mergeCell ref="AF32:AI32"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="E33:H33"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="N33:Q33"/>
     <mergeCell ref="S33:V33"/>
+    <mergeCell ref="W33:Z33"/>
     <mergeCell ref="AB33:AE33"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="AF33:AI33"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="J32:M32"/>
     <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:Z32"/>
+    <mergeCell ref="AB29:AE29"/>
+    <mergeCell ref="AF29:AI29"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="J30:M30"/>
     <mergeCell ref="N30:Q30"/>
     <mergeCell ref="S30:V30"/>
+    <mergeCell ref="W30:Z30"/>
     <mergeCell ref="AB30:AE30"/>
-    <mergeCell ref="AB28:AE28"/>
-    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="AF30:AI30"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="J29:M29"/>
     <mergeCell ref="N29:Q29"/>
     <mergeCell ref="S29:V29"/>
     <mergeCell ref="W29:Z29"/>
-    <mergeCell ref="AB29:AE29"/>
-    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="AF27:AI27"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="J28:M28"/>
     <mergeCell ref="N28:Q28"/>
     <mergeCell ref="S28:V28"/>
     <mergeCell ref="W28:Z28"/>
-    <mergeCell ref="AB26:AE26"/>
-    <mergeCell ref="AF26:AI26"/>
+    <mergeCell ref="AB28:AE28"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="W25:Z25"/>
+    <mergeCell ref="AB25:AE25"/>
+    <mergeCell ref="AF25:AI25"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="J27:M27"/>
@@ -10576,64 +10892,54 @@
     <mergeCell ref="S27:V27"/>
     <mergeCell ref="W27:Z27"/>
     <mergeCell ref="AB27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="AB24:AE24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="S24:V24"/>
+    <mergeCell ref="W24:Z24"/>
     <mergeCell ref="AF24:AI24"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="J25:M25"/>
     <mergeCell ref="N25:Q25"/>
     <mergeCell ref="S25:V25"/>
-    <mergeCell ref="W25:Z25"/>
-    <mergeCell ref="AB25:AE25"/>
-    <mergeCell ref="AF25:AI25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="S24:V24"/>
-    <mergeCell ref="W24:Z24"/>
+    <mergeCell ref="AB22:AE22"/>
     <mergeCell ref="AF22:AI22"/>
-    <mergeCell ref="A23:D23"/>
     <mergeCell ref="E23:H23"/>
-    <mergeCell ref="J23:M23"/>
     <mergeCell ref="N23:Q23"/>
     <mergeCell ref="S23:V23"/>
     <mergeCell ref="W23:Z23"/>
-    <mergeCell ref="AB23:AE23"/>
     <mergeCell ref="AF23:AI23"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="AB21:AE21"/>
-    <mergeCell ref="AF21:AI21"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="N22:Q22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="W22:Z22"/>
-    <mergeCell ref="AB22:AE22"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="W20:Z20"/>
+    <mergeCell ref="AB20:AE20"/>
     <mergeCell ref="AF20:AI20"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="J21:M21"/>
     <mergeCell ref="N21:Q21"/>
     <mergeCell ref="S21:V21"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="AB21:AE21"/>
+    <mergeCell ref="AF21:AI21"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="W20:Z20"/>
     <mergeCell ref="AB18:AE18"/>
     <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="A19:D19"/>
     <mergeCell ref="E19:H19"/>
+    <mergeCell ref="J19:M19"/>
     <mergeCell ref="N19:Q19"/>
     <mergeCell ref="S19:V19"/>
     <mergeCell ref="W19:Z19"/>
+    <mergeCell ref="AB19:AE19"/>
     <mergeCell ref="AF19:AI19"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="E18:H18"/>
@@ -10641,38 +10947,6 @@
     <mergeCell ref="N18:Q18"/>
     <mergeCell ref="S18:V18"/>
     <mergeCell ref="W18:Z18"/>
-    <mergeCell ref="AB16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="S17:V17"/>
-    <mergeCell ref="W17:Z17"/>
-    <mergeCell ref="AB17:AE17"/>
-    <mergeCell ref="AF17:AI17"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="S16:V16"/>
-    <mergeCell ref="W16:Z16"/>
-    <mergeCell ref="AB14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="S15:V15"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="AB15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W14:Z14"/>
     <mergeCell ref="AB12:AE12"/>
     <mergeCell ref="AF12:AI12"/>
     <mergeCell ref="A13:D13"/>

</xml_diff>